<commit_message>
Corrected Employees work hours
</commit_message>
<xml_diff>
--- a/config_files/Horarios/Medibiofarma/Horacio Moreno.xlsx
+++ b/config_files/Horarios/Medibiofarma/Horacio Moreno.xlsx
@@ -4676,7 +4676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="494">
+  <cellXfs count="500">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5813,6 +5813,24 @@
     </xf>
     <xf numFmtId="14" fontId="473" fillId="15" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment horizontal="center"/>
@@ -11259,11 +11277,11 @@
       <c r="B18" s="115">
         <v>3</v>
       </c>
-      <c r="C18" s="387">
+      <c r="C18" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E18" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E18" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G18" s="113">
         <f>((E18-C18)*24)</f>
@@ -11274,11 +11292,11 @@
       <c r="B19" s="115">
         <v>4</v>
       </c>
-      <c r="C19" s="387">
+      <c r="C19" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E19" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E19" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G19" s="113">
         <f>((E19-C19)*24)</f>
@@ -11289,11 +11307,11 @@
       <c r="B20" s="115">
         <v>5</v>
       </c>
-      <c r="C20" s="387">
+      <c r="C20" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E20" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E20" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G20" s="113">
         <f>((E20-C20)*24)</f>
@@ -11314,11 +11332,11 @@
       <c r="B22" s="115">
         <v>7</v>
       </c>
-      <c r="C22" s="387">
+      <c r="C22" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E22" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E22" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G22" s="113">
         <f>((E22-C22)*24)</f>
@@ -11349,11 +11367,11 @@
       <c r="B25" s="115">
         <v>10</v>
       </c>
-      <c r="C25" s="387">
+      <c r="C25" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E25" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E25" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G25" s="113">
         <f>((E25-C25)*24)</f>
@@ -11364,11 +11382,11 @@
       <c r="B26" s="115">
         <v>11</v>
       </c>
-      <c r="C26" s="387">
+      <c r="C26" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E26" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E26" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G26" s="113">
         <f>((E26-C26)*24)</f>
@@ -11379,11 +11397,11 @@
       <c r="B27" s="115">
         <v>12</v>
       </c>
-      <c r="C27" s="387">
+      <c r="C27" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E27" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E27" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G27" s="113">
         <f>((E27-C27)*24)</f>
@@ -11394,11 +11412,11 @@
       <c r="B28" s="115">
         <v>13</v>
       </c>
-      <c r="C28" s="387">
+      <c r="C28" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E28" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E28" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G28" s="113">
         <f>((E28-C28)*24)</f>
@@ -11409,11 +11427,11 @@
       <c r="B29" s="115">
         <v>14</v>
       </c>
-      <c r="C29" s="387">
+      <c r="C29" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E29" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E29" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G29" s="113">
         <f>((E29-C29)*24)</f>
@@ -11444,11 +11462,11 @@
       <c r="B32" s="115">
         <v>17</v>
       </c>
-      <c r="C32" s="387">
+      <c r="C32" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E32" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E32" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G32" s="113">
         <f>((E32-C32)*24)</f>
@@ -11459,11 +11477,11 @@
       <c r="B33" s="115">
         <v>18</v>
       </c>
-      <c r="C33" s="387">
+      <c r="C33" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E33" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E33" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G33" s="113">
         <f>((E33-C33)*24)</f>
@@ -11474,11 +11492,11 @@
       <c r="B34" s="115">
         <v>19</v>
       </c>
-      <c r="C34" s="387">
+      <c r="C34" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E34" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E34" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G34" s="113">
         <f>((E34-C34)*24)</f>
@@ -11489,11 +11507,11 @@
       <c r="B35" s="115">
         <v>20</v>
       </c>
-      <c r="C35" s="387">
+      <c r="C35" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E35" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E35" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G35" s="113">
         <f>((E35-C35)*24)</f>
@@ -11504,11 +11522,11 @@
       <c r="B36" s="115">
         <v>21</v>
       </c>
-      <c r="C36" s="387">
+      <c r="C36" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E36" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E36" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G36" s="113">
         <f>((E36-C36)*24)</f>
@@ -11539,11 +11557,11 @@
       <c r="B39" s="115">
         <v>24</v>
       </c>
-      <c r="C39" s="387">
+      <c r="C39" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E39" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E39" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G39" s="113">
         <f>((E39-C39)*24)</f>
@@ -11554,11 +11572,11 @@
       <c r="B40" s="115">
         <v>25</v>
       </c>
-      <c r="C40" s="387">
+      <c r="C40" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E40" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E40" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G40" s="113">
         <f>((E40-C40)*24)</f>
@@ -11569,11 +11587,11 @@
       <c r="B41" s="115">
         <v>26</v>
       </c>
-      <c r="C41" s="387">
+      <c r="C41" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E41" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E41" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G41" s="113">
         <f>((E41-C41)*24)</f>
@@ -11584,11 +11602,11 @@
       <c r="B42" s="115">
         <v>27</v>
       </c>
-      <c r="C42" s="387">
+      <c r="C42" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E42" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E42" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G42" s="113">
         <f>((E42-C42)*24)</f>
@@ -11599,11 +11617,11 @@
       <c r="B43" s="115">
         <v>28</v>
       </c>
-      <c r="C43" s="387">
+      <c r="C43" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E43" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E43" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G43" s="113">
         <f>((E43-C43)*24)</f>
@@ -11634,11 +11652,11 @@
       <c r="B46" s="115">
         <v>31</v>
       </c>
-      <c r="C46" s="387">
+      <c r="C46" s="498" t="n">
         <v>0.375</v>
       </c>
-      <c r="E46" s="387">
-        <v>0.54166666666666663</v>
+      <c r="E46" s="498" t="n">
+        <v>0.5416666666666666</v>
       </c>
       <c r="G46" s="113">
         <f>((E46-C46)*24)</f>
@@ -11740,6 +11758,7 @@
       <c r="H62" s="397"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="B58:H62"/>
     <mergeCell ref="B6:H6"/>
@@ -12417,6 +12436,7 @@
       <c r="H62" s="407"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="B58:H62"/>
@@ -13117,6 +13137,7 @@
       <c r="H62" s="413"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="B58:H62"/>
     <mergeCell ref="B6:H6"/>
@@ -13305,8 +13326,12 @@
       <c r="B16" s="189">
         <v>1</v>
       </c>
-      <c r="C16" s="190"/>
-      <c r="E16" s="190"/>
+      <c r="C16" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E16" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G16" s="187">
         <f>((E16-C16)*24)</f>
         <v>0</v>
@@ -13336,8 +13361,12 @@
       <c r="B19" s="189">
         <v>4</v>
       </c>
-      <c r="C19" s="190"/>
-      <c r="E19" s="190"/>
+      <c r="C19" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E19" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G19" s="187">
         <f>((E19-C19)*24)</f>
         <v>0</v>
@@ -13347,8 +13376,12 @@
       <c r="B20" s="189">
         <v>5</v>
       </c>
-      <c r="C20" s="190"/>
-      <c r="E20" s="190"/>
+      <c r="C20" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E20" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G20" s="187">
         <f>((E20-C20)*24)</f>
         <v>0</v>
@@ -13358,8 +13391,12 @@
       <c r="B21" s="189">
         <v>6</v>
       </c>
-      <c r="C21" s="190"/>
-      <c r="E21" s="190"/>
+      <c r="C21" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E21" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G21" s="187">
         <f>((E21-C21)*24)</f>
         <v>0</v>
@@ -13369,8 +13406,12 @@
       <c r="B22" s="189">
         <v>7</v>
       </c>
-      <c r="C22" s="190"/>
-      <c r="E22" s="190"/>
+      <c r="C22" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E22" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G22" s="187">
         <f>((E22-C22)*24)</f>
         <v>0</v>
@@ -13380,8 +13421,12 @@
       <c r="B23" s="189">
         <v>8</v>
       </c>
-      <c r="C23" s="190"/>
-      <c r="E23" s="190"/>
+      <c r="C23" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E23" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G23" s="187">
         <f>((E23-C23)*24)</f>
         <v>0</v>
@@ -13411,8 +13456,12 @@
       <c r="B26" s="189">
         <v>11</v>
       </c>
-      <c r="C26" s="190"/>
-      <c r="E26" s="190"/>
+      <c r="C26" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E26" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G26" s="187">
         <f>((E26-C26)*24)</f>
         <v>0</v>
@@ -13422,8 +13471,12 @@
       <c r="B27" s="189">
         <v>12</v>
       </c>
-      <c r="C27" s="190"/>
-      <c r="E27" s="190"/>
+      <c r="C27" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E27" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G27" s="187">
         <f>((E27-C27)*24)</f>
         <v>0</v>
@@ -13433,8 +13486,12 @@
       <c r="B28" s="189">
         <v>13</v>
       </c>
-      <c r="C28" s="190"/>
-      <c r="E28" s="190"/>
+      <c r="C28" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E28" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G28" s="187">
         <f>((E28-C28)*24)</f>
         <v>0</v>
@@ -13494,8 +13551,12 @@
       <c r="B34" s="189">
         <v>19</v>
       </c>
-      <c r="C34" s="190"/>
-      <c r="E34" s="190"/>
+      <c r="C34" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E34" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G34" s="187">
         <f>((E34-C34)*24)</f>
         <v>0</v>
@@ -13505,8 +13566,12 @@
       <c r="B35" s="189">
         <v>20</v>
       </c>
-      <c r="C35" s="190"/>
-      <c r="E35" s="190"/>
+      <c r="C35" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E35" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G35" s="187">
         <f>((E35-C35)*24)</f>
         <v>0</v>
@@ -13516,8 +13581,12 @@
       <c r="B36" s="189">
         <v>21</v>
       </c>
-      <c r="C36" s="190"/>
-      <c r="E36" s="190"/>
+      <c r="C36" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E36" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G36" s="187">
         <f>((E36-C36)*24)</f>
         <v>0</v>
@@ -13527,8 +13596,12 @@
       <c r="B37" s="189">
         <v>22</v>
       </c>
-      <c r="C37" s="190"/>
-      <c r="E37" s="190"/>
+      <c r="C37" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E37" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G37" s="187">
         <f>((E37-C37)*24)</f>
         <v>0</v>
@@ -13558,8 +13631,12 @@
       <c r="B40" s="189">
         <v>25</v>
       </c>
-      <c r="C40" s="190"/>
-      <c r="E40" s="190"/>
+      <c r="C40" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E40" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G40" s="187">
         <f>((E40-C40)*24)</f>
         <v>0</v>
@@ -13569,8 +13646,12 @@
       <c r="B41" s="189">
         <v>26</v>
       </c>
-      <c r="C41" s="190"/>
-      <c r="E41" s="190"/>
+      <c r="C41" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E41" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G41" s="187">
         <f>((E41-C41)*24)</f>
         <v>0</v>
@@ -13580,8 +13661,12 @@
       <c r="B42" s="189">
         <v>27</v>
       </c>
-      <c r="C42" s="190"/>
-      <c r="E42" s="190"/>
+      <c r="C42" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E42" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G42" s="187">
         <f>((E42-C42)*24)</f>
         <v>0</v>
@@ -13591,8 +13676,12 @@
       <c r="B43" s="189">
         <v>28</v>
       </c>
-      <c r="C43" s="190"/>
-      <c r="E43" s="190"/>
+      <c r="C43" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E43" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G43" s="187">
         <f>((E43-C43)*24)</f>
         <v>0</v>
@@ -13602,8 +13691,12 @@
       <c r="B44" s="189">
         <v>29</v>
       </c>
-      <c r="C44" s="190"/>
-      <c r="E44" s="190"/>
+      <c r="C44" s="495" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E44" s="495" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G44" s="187">
         <f>((E44-C44)*24)</f>
         <v>0</v>
@@ -13713,6 +13806,7 @@
       <c r="H62" s="421"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="B58:H62"/>
     <mergeCell ref="B6:H6"/>
@@ -13911,8 +14005,12 @@
       <c r="B17" s="214">
         <v>2</v>
       </c>
-      <c r="C17" s="215"/>
-      <c r="E17" s="215"/>
+      <c r="C17" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E17" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G17" s="212">
         <f>((E17-C17)*24)</f>
         <v>0</v>
@@ -13922,8 +14020,12 @@
       <c r="B18" s="214">
         <v>3</v>
       </c>
-      <c r="C18" s="215"/>
-      <c r="E18" s="215"/>
+      <c r="C18" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E18" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G18" s="212">
         <f>((E18-C18)*24)</f>
         <v>0</v>
@@ -13933,8 +14035,12 @@
       <c r="B19" s="214">
         <v>4</v>
       </c>
-      <c r="C19" s="215"/>
-      <c r="E19" s="215"/>
+      <c r="C19" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E19" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G19" s="212">
         <f>((E19-C19)*24)</f>
         <v>0</v>
@@ -13944,8 +14050,12 @@
       <c r="B20" s="214">
         <v>5</v>
       </c>
-      <c r="C20" s="215"/>
-      <c r="E20" s="215"/>
+      <c r="C20" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E20" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G20" s="212">
         <f>((E20-C20)*24)</f>
         <v>0</v>
@@ -13955,8 +14065,12 @@
       <c r="B21" s="214">
         <v>6</v>
       </c>
-      <c r="C21" s="215"/>
-      <c r="E21" s="215"/>
+      <c r="C21" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E21" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G21" s="212">
         <f>((E21-C21)*24)</f>
         <v>0</v>
@@ -13986,8 +14100,12 @@
       <c r="B24" s="214">
         <v>9</v>
       </c>
-      <c r="C24" s="215"/>
-      <c r="E24" s="215"/>
+      <c r="C24" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E24" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G24" s="212">
         <f>((E24-C24)*24)</f>
         <v>0</v>
@@ -13997,8 +14115,12 @@
       <c r="B25" s="214">
         <v>10</v>
       </c>
-      <c r="C25" s="215"/>
-      <c r="E25" s="215"/>
+      <c r="C25" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E25" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G25" s="212">
         <f>((E25-C25)*24)</f>
         <v>0</v>
@@ -14008,8 +14130,12 @@
       <c r="B26" s="214">
         <v>11</v>
       </c>
-      <c r="C26" s="215"/>
-      <c r="E26" s="215"/>
+      <c r="C26" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E26" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G26" s="212">
         <f>((E26-C26)*24)</f>
         <v>0</v>
@@ -14019,8 +14145,12 @@
       <c r="B27" s="214">
         <v>12</v>
       </c>
-      <c r="C27" s="215"/>
-      <c r="E27" s="215"/>
+      <c r="C27" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E27" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G27" s="212">
         <f>((E27-C27)*24)</f>
         <v>0</v>
@@ -14030,8 +14160,12 @@
       <c r="B28" s="214">
         <v>13</v>
       </c>
-      <c r="C28" s="215"/>
-      <c r="E28" s="215"/>
+      <c r="C28" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E28" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G28" s="212">
         <f>((E28-C28)*24)</f>
         <v>0</v>
@@ -14061,8 +14195,12 @@
       <c r="B31" s="214">
         <v>16</v>
       </c>
-      <c r="C31" s="215"/>
-      <c r="E31" s="215"/>
+      <c r="C31" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E31" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G31" s="212">
         <f>((E31-C31)*24)</f>
         <v>0</v>
@@ -14072,8 +14210,12 @@
       <c r="B32" s="214">
         <v>17</v>
       </c>
-      <c r="C32" s="215"/>
-      <c r="E32" s="215"/>
+      <c r="C32" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E32" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G32" s="212">
         <f>((E32-C32)*24)</f>
         <v>0</v>
@@ -14083,8 +14225,12 @@
       <c r="B33" s="214">
         <v>18</v>
       </c>
-      <c r="C33" s="215"/>
-      <c r="E33" s="215"/>
+      <c r="C33" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E33" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G33" s="212">
         <f>((E33-C33)*24)</f>
         <v>0</v>
@@ -14094,8 +14240,12 @@
       <c r="B34" s="214">
         <v>19</v>
       </c>
-      <c r="C34" s="215"/>
-      <c r="E34" s="215"/>
+      <c r="C34" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E34" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G34" s="212">
         <f>((E34-C34)*24)</f>
         <v>0</v>
@@ -14105,8 +14255,12 @@
       <c r="B35" s="214">
         <v>20</v>
       </c>
-      <c r="C35" s="215"/>
-      <c r="E35" s="215"/>
+      <c r="C35" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E35" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G35" s="212">
         <f>((E35-C35)*24)</f>
         <v>0</v>
@@ -14136,8 +14290,12 @@
       <c r="B38" s="214">
         <v>23</v>
       </c>
-      <c r="C38" s="215"/>
-      <c r="E38" s="215"/>
+      <c r="C38" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E38" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G38" s="212">
         <f>((E38-C38)*24)</f>
         <v>0</v>
@@ -14147,8 +14305,12 @@
       <c r="B39" s="214">
         <v>24</v>
       </c>
-      <c r="C39" s="215"/>
-      <c r="E39" s="215"/>
+      <c r="C39" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E39" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G39" s="212">
         <f>((E39-C39)*24)</f>
         <v>0</v>
@@ -14158,8 +14320,12 @@
       <c r="B40" s="214">
         <v>25</v>
       </c>
-      <c r="C40" s="215"/>
-      <c r="E40" s="215"/>
+      <c r="C40" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E40" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G40" s="212">
         <f>((E40-C40)*24)</f>
         <v>0</v>
@@ -14169,8 +14335,12 @@
       <c r="B41" s="214">
         <v>26</v>
       </c>
-      <c r="C41" s="215"/>
-      <c r="E41" s="215"/>
+      <c r="C41" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E41" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G41" s="212">
         <f>((E41-C41)*24)</f>
         <v>0</v>
@@ -14180,8 +14350,12 @@
       <c r="B42" s="214">
         <v>27</v>
       </c>
-      <c r="C42" s="215"/>
-      <c r="E42" s="215"/>
+      <c r="C42" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E42" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G42" s="212">
         <f>((E42-C42)*24)</f>
         <v>0</v>
@@ -14211,8 +14385,12 @@
       <c r="B45" s="214">
         <v>30</v>
       </c>
-      <c r="C45" s="215"/>
-      <c r="E45" s="215"/>
+      <c r="C45" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E45" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G45" s="212">
         <f>((E45-C45)*24)</f>
         <v>0</v>
@@ -14222,8 +14400,12 @@
       <c r="B46" s="214">
         <v>31</v>
       </c>
-      <c r="C46" s="215"/>
-      <c r="E46" s="215"/>
+      <c r="C46" s="496" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E46" s="496" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G46" s="212">
         <f>((E46-C46)*24)</f>
         <v>0</v>
@@ -14318,6 +14500,7 @@
       <c r="H62" s="429"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="B58:H62"/>
     <mergeCell ref="B6:H6"/>
@@ -14496,8 +14679,12 @@
       <c r="B16" s="238">
         <v>1</v>
       </c>
-      <c r="C16" s="239"/>
-      <c r="E16" s="239"/>
+      <c r="C16" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E16" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G16" s="236">
         <f>((E16-C16)*24)</f>
         <v>0</v>
@@ -14507,8 +14694,12 @@
       <c r="B17" s="238">
         <v>2</v>
       </c>
-      <c r="C17" s="239"/>
-      <c r="E17" s="239"/>
+      <c r="C17" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E17" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G17" s="236">
         <f>((E17-C17)*24)</f>
         <v>0</v>
@@ -14518,8 +14709,12 @@
       <c r="B18" s="238">
         <v>3</v>
       </c>
-      <c r="C18" s="239"/>
-      <c r="E18" s="239"/>
+      <c r="C18" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E18" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G18" s="236">
         <f>((E18-C18)*24)</f>
         <v>0</v>
@@ -14549,8 +14744,12 @@
       <c r="B21" s="238">
         <v>6</v>
       </c>
-      <c r="C21" s="239"/>
-      <c r="E21" s="239"/>
+      <c r="C21" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E21" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G21" s="236">
         <f>((E21-C21)*24)</f>
         <v>0</v>
@@ -14560,8 +14759,12 @@
       <c r="B22" s="238">
         <v>7</v>
       </c>
-      <c r="C22" s="239"/>
-      <c r="E22" s="239"/>
+      <c r="C22" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E22" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G22" s="236">
         <f>((E22-C22)*24)</f>
         <v>0</v>
@@ -14571,8 +14774,12 @@
       <c r="B23" s="238">
         <v>8</v>
       </c>
-      <c r="C23" s="239"/>
-      <c r="E23" s="239"/>
+      <c r="C23" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E23" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G23" s="236">
         <f>((E23-C23)*24)</f>
         <v>0</v>
@@ -14582,8 +14789,12 @@
       <c r="B24" s="238">
         <v>9</v>
       </c>
-      <c r="C24" s="239"/>
-      <c r="E24" s="239"/>
+      <c r="C24" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E24" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G24" s="236">
         <f>((E24-C24)*24)</f>
         <v>0</v>
@@ -14593,8 +14804,12 @@
       <c r="B25" s="238">
         <v>10</v>
       </c>
-      <c r="C25" s="239"/>
-      <c r="E25" s="239"/>
+      <c r="C25" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E25" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G25" s="236">
         <f>((E25-C25)*24)</f>
         <v>0</v>
@@ -14624,8 +14839,12 @@
       <c r="B28" s="238">
         <v>13</v>
       </c>
-      <c r="C28" s="239"/>
-      <c r="E28" s="239"/>
+      <c r="C28" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E28" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G28" s="236">
         <f>((E28-C28)*24)</f>
         <v>0</v>
@@ -14635,8 +14854,12 @@
       <c r="B29" s="238">
         <v>14</v>
       </c>
-      <c r="C29" s="239"/>
-      <c r="E29" s="239"/>
+      <c r="C29" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E29" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G29" s="236">
         <f>((E29-C29)*24)</f>
         <v>0</v>
@@ -14646,8 +14869,12 @@
       <c r="B30" s="238">
         <v>15</v>
       </c>
-      <c r="C30" s="239"/>
-      <c r="E30" s="239"/>
+      <c r="C30" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E30" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G30" s="236">
         <f>((E30-C30)*24)</f>
         <v>0</v>
@@ -14657,8 +14884,12 @@
       <c r="B31" s="238">
         <v>16</v>
       </c>
-      <c r="C31" s="239"/>
-      <c r="E31" s="239"/>
+      <c r="C31" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E31" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G31" s="236">
         <f>((E31-C31)*24)</f>
         <v>0</v>
@@ -14668,8 +14899,12 @@
       <c r="B32" s="238">
         <v>17</v>
       </c>
-      <c r="C32" s="239"/>
-      <c r="E32" s="239"/>
+      <c r="C32" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E32" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G32" s="236">
         <f>((E32-C32)*24)</f>
         <v>0</v>
@@ -14699,8 +14934,12 @@
       <c r="B35" s="238">
         <v>20</v>
       </c>
-      <c r="C35" s="239"/>
-      <c r="E35" s="239"/>
+      <c r="C35" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E35" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G35" s="236">
         <f>((E35-C35)*24)</f>
         <v>0</v>
@@ -14710,8 +14949,12 @@
       <c r="B36" s="238">
         <v>21</v>
       </c>
-      <c r="C36" s="239"/>
-      <c r="E36" s="239"/>
+      <c r="C36" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E36" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G36" s="236">
         <f>((E36-C36)*24)</f>
         <v>0</v>
@@ -14721,8 +14964,12 @@
       <c r="B37" s="238">
         <v>22</v>
       </c>
-      <c r="C37" s="239"/>
-      <c r="E37" s="239"/>
+      <c r="C37" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E37" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G37" s="236">
         <f>((E37-C37)*24)</f>
         <v>0</v>
@@ -14732,8 +14979,12 @@
       <c r="B38" s="238">
         <v>23</v>
       </c>
-      <c r="C38" s="239"/>
-      <c r="E38" s="239"/>
+      <c r="C38" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E38" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G38" s="236">
         <f>((E38-C38)*24)</f>
         <v>0</v>
@@ -14743,8 +14994,12 @@
       <c r="B39" s="238">
         <v>24</v>
       </c>
-      <c r="C39" s="239"/>
-      <c r="E39" s="239"/>
+      <c r="C39" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E39" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G39" s="236">
         <f>((E39-C39)*24)</f>
         <v>0</v>
@@ -14774,8 +15029,12 @@
       <c r="B42" s="238">
         <v>27</v>
       </c>
-      <c r="C42" s="239"/>
-      <c r="E42" s="239"/>
+      <c r="C42" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E42" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G42" s="236">
         <f>((E42-C42)*24)</f>
         <v>0</v>
@@ -14785,8 +15044,12 @@
       <c r="B43" s="238">
         <v>28</v>
       </c>
-      <c r="C43" s="239"/>
-      <c r="E43" s="239"/>
+      <c r="C43" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E43" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G43" s="236">
         <f>((E43-C43)*24)</f>
         <v>0</v>
@@ -14796,8 +15059,12 @@
       <c r="B44" s="238">
         <v>29</v>
       </c>
-      <c r="C44" s="239"/>
-      <c r="E44" s="239"/>
+      <c r="C44" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E44" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G44" s="236">
         <f>((E44-C44)*24)</f>
         <v>0</v>
@@ -14807,8 +15074,12 @@
       <c r="B45" s="238">
         <v>30</v>
       </c>
-      <c r="C45" s="239"/>
-      <c r="E45" s="239"/>
+      <c r="C45" s="499" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E45" s="499" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="G45" s="236">
         <f>((E45-C45)*24)</f>
         <v>0</v>
@@ -14903,6 +15174,7 @@
       <c r="H62" s="437"/>
     </row>
   </sheetData>
+  <sheetProtection password="BCDB" sheet="true" scenarios="true" objects="true"/>
   <mergeCells count="7">
     <mergeCell ref="B58:H62"/>
     <mergeCell ref="B6:H6"/>

</xml_diff>